<commit_message>
# Update my log.
</commit_message>
<xml_diff>
--- a/c1/trainrec.xlsx
+++ b/c1/trainrec.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="14940" windowHeight="9450"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="14940" windowHeight="9450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>培训阶段</t>
   </si>
@@ -329,6 +330,63 @@
       <t xml:space="preserve"> </t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天7:31 2011-04-01查我的学车资料状态已经是已结业了</t>
+  </si>
+  <si>
+    <t>[查看]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 张昀</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 已结业</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 初次申请</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2010-10-25 00:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 广州市穗通驾驶员培训有限公司</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JP440106000014</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> S10111016</t>
+  </si>
+  <si>
+    <t>当前处于阶段</t>
+  </si>
+  <si>
+    <t>大纲要求培训时长为:</t>
+  </si>
+  <si>
+    <t>实操</t>
+  </si>
+  <si>
+    <t>实际完成：</t>
+  </si>
+  <si>
+    <t>学员名称</t>
+  </si>
+  <si>
+    <t>培训车型</t>
+  </si>
+  <si>
+    <t>培训状态</t>
+  </si>
+  <si>
+    <t>培训类型</t>
+  </si>
+  <si>
+    <t>入学时间</t>
   </si>
 </sst>
 </file>
@@ -773,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -1520,4 +1578,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
# update some log.
</commit_message>
<xml_diff>
--- a/c1/trainrec.xlsx
+++ b/c1/trainrec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="14940" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="14940" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -831,13 +831,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30">
@@ -1584,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>